<commit_message>
Extended the email functionaltiy and bug fixes
</commit_message>
<xml_diff>
--- a/config/NMRA_Email_Distribution_List_Template.xlsx
+++ b/config/NMRA_Email_Distribution_List_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erich/Documents/GitHub/Personal/NMRAMembers/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE33D1A-7841-D349-98D1-45E64D287F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8AA9EB-3A70-7E4C-A941-BDB55F09E3C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="69760" yWindow="-13860" windowWidth="40540" windowHeight="19040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="69760" yWindow="-13860" windowWidth="40540" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Email Distribution" sheetId="2" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>email_address</t>
   </si>
   <si>
-    <t>zip_file</t>
-  </si>
-  <si>
     <t>NMRA</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>jack@somewhere.com</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>This sends just the person's division file</t>
   </si>
   <si>
@@ -108,6 +102,12 @@
   </si>
   <si>
     <t>smtp.somewhere.com</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D51535-F360-A949-9F57-A1DCBE9827E6}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -579,15 +579,15 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -596,24 +596,24 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -622,24 +622,24 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -648,19 +648,19 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -677,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34207A20-5CA3-0849-A10C-B60A7CA70C32}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -701,11 +701,11 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>